<commit_message>
Freeze Bulk QR Code with additional functionality
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GenAI Projects\qr-code-generator-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C12BB2-4219-4265-BEBC-FCF3E5ACEC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF7E21C-0476-4F7E-B3E3-DEA4365788E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8BF9E950-9155-4008-9F92-CD3259CD626A}"/>
   </bookViews>
@@ -37,38 +37,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>AI ROBO HUB</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>https://airobohub.com</t>
   </si>
   <si>
-    <t>FTS</t>
-  </si>
-  <si>
     <t>https://futuretechsolution.in</t>
   </si>
   <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
     <t>https://microsoft.com</t>
   </si>
   <si>
-    <t>OpenAI</t>
-  </si>
-  <si>
     <t>https://openai.com</t>
   </si>
   <si>
-    <t>AI Studio</t>
-  </si>
-  <si>
     <t>https://aistudio.google.com</t>
   </si>
   <si>
@@ -78,7 +60,7 @@
     <t>pending</t>
   </si>
   <si>
-    <t>company_name</t>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -431,82 +413,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A2E527-83C2-428E-BEF5-5DA3918D075F}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>